<commit_message>
Refactor date range calculation and improve navigation logic in date picker
</commit_message>
<xml_diff>
--- a/reservations_2025-02-25T16-12-51-458Z.xlsx
+++ b/reservations_2025-02-25T16-12-51-458Z.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Reservations"/>
+    <sheet name="Reservations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -763,15 +780,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="2">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -794,25 +819,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -821,10 +838,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -862,71 +879,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -950,53 +967,50 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1006,7 +1020,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1015,7 +1029,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1024,7 +1038,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1032,10 +1046,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1064,7 +1078,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -1077,12 +1091,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -1094,36 +1109,74 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="1">
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="2" max="2" width="31.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="3" max="3" width="22.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="4" max="4" width="18.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="5" max="5" width="18.625" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="6" max="6" width="33.625" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="7" max="7" width="24.25" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="8" max="8" width="10.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="9" max="9" width="10.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="10" max="10" width="10.875" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="11" max="11" width="23.5" customWidth="1" level="0" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1240,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1220,7 +1273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1249,7 +1302,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1278,7 +1331,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1307,7 +1360,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1336,7 +1389,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -1365,7 +1418,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1394,7 +1447,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1423,7 +1476,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1452,7 +1505,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
@@ -1481,7 +1534,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -1510,7 +1563,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -1539,7 +1592,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1568,7 +1621,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
@@ -1597,7 +1650,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -1626,7 +1679,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>88</v>
       </c>
@@ -1655,7 +1708,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>91</v>
       </c>
@@ -1684,7 +1737,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -1713,7 +1766,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -1742,7 +1795,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" ht="17.25" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>100</v>
       </c>
@@ -1771,7 +1824,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" ht="17.25" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -1800,7 +1853,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" ht="17.25" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>100</v>
       </c>
@@ -1829,7 +1882,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" ht="17.25" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>110</v>
       </c>
@@ -1862,7 +1915,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" ht="17.25" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
@@ -1891,7 +1944,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" ht="17.25" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>122</v>
       </c>
@@ -1920,7 +1973,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" ht="17.25" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>122</v>
       </c>
@@ -1949,7 +2002,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" ht="17.25" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>130</v>
       </c>
@@ -1982,7 +2035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" ht="17.25" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>136</v>
       </c>
@@ -2011,7 +2064,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" ht="17.25" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>141</v>
       </c>
@@ -2040,7 +2093,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32" ht="17.25" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>144</v>
       </c>
@@ -2069,7 +2122,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row r="33" ht="17.25" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>149</v>
       </c>
@@ -2098,7 +2151,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row r="34" ht="17.25" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -2127,7 +2180,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row r="35" ht="17.25" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>159</v>
       </c>
@@ -2156,7 +2209,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row r="36" ht="17.25" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>163</v>
       </c>
@@ -2185,7 +2238,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="37" ht="17.25" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>166</v>
       </c>
@@ -2214,7 +2267,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row r="38" ht="17.25" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>170</v>
       </c>
@@ -2243,7 +2296,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row r="39" ht="17.25" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -2272,7 +2325,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row r="40" ht="17.25" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>178</v>
       </c>
@@ -2301,7 +2354,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row r="41" ht="17.25" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>183</v>
       </c>
@@ -2330,7 +2383,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row r="42" ht="17.25" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>188</v>
       </c>
@@ -2363,7 +2416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row r="43" ht="17.25" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>194</v>
       </c>
@@ -2392,7 +2445,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row r="44" ht="17.25" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>183</v>
       </c>
@@ -2421,7 +2474,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row r="45" ht="17.25" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>201</v>
       </c>
@@ -2450,7 +2503,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row r="46" ht="17.25" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>205</v>
       </c>
@@ -2479,7 +2532,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row r="47" ht="17.25" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>209</v>
       </c>
@@ -2508,7 +2561,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row r="48" ht="17.25" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>213</v>
       </c>
@@ -2537,7 +2590,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row r="49" ht="17.25" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>174</v>
       </c>
@@ -2566,7 +2619,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+    <row r="50" ht="17.25" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>220</v>
       </c>
@@ -2595,7 +2648,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+    <row r="51" ht="17.25" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>225</v>
       </c>
@@ -2624,7 +2677,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+    <row r="52" ht="17.25" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>228</v>
       </c>
@@ -2653,7 +2706,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+    <row r="53" ht="17.25" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>232</v>
       </c>
@@ -2682,7 +2735,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+    <row r="54" ht="17.25" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>236</v>
       </c>
@@ -2711,7 +2764,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+    <row r="55" ht="17.25" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>240</v>
       </c>
@@ -2740,7 +2793,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+    <row r="56" ht="17.25" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>244</v>
       </c>
@@ -2770,6 +2823,8 @@
       <c r="K56" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K56"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>